<commit_message>
4 passed 2 failed
</commit_message>
<xml_diff>
--- a/test_data/Copy of pharmeasy.xlsx
+++ b/test_data/Copy of pharmeasy.xlsx
@@ -168,7 +168,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -180,12 +180,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -484,7 +478,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -497,10 +491,10 @@
       <c r="A1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -508,32 +502,32 @@
       <c r="A2" s="1">
         <v>577301</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="1">
         <v>9008240114</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="7">
+      <c r="A3" s="1">
         <v>572222</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="1">
         <v>8217374794</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="7">
-        <v>560001</v>
-      </c>
-      <c r="B4" s="7" t="s">
+      <c r="A4" s="1">
+        <v>111</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="1">
         <v>9008240114</v>
       </c>
     </row>

</xml_diff>